<commit_message>
finished bf3 and updated bf2 3 panel graph to include sub-captions
</commit_message>
<xml_diff>
--- a/data/toothpaste_bf3.xlsx
+++ b/data/toothpaste_bf3.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/Math326DoE/Math326_Quarto4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{21E5E020-E692-4850-93C8-30C9975FB5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C065FEE-2CAD-49B3-A478-29BE87771DBA}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{21E5E020-E692-4850-93C8-30C9975FB5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6F36236-64A1-455B-89EA-F34B85B57D3E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
     <sheet name="BF1_decomp" sheetId="5" r:id="rId2"/>
     <sheet name="ToothbrushStudy_Data" sheetId="1" r:id="rId3"/>
     <sheet name="attractive" sheetId="8" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
-    <sheet name="lifeboat" sheetId="7" r:id="rId8"/>
+    <sheet name="attractive_decomp" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId8"/>
+    <sheet name="lifeboat" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="174">
   <si>
     <t>Brush</t>
   </si>
@@ -1329,6 +1330,34 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>obs number (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -2387,7 +2416,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2607,75 +2636,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="33" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="25" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2734,7 +2694,75 @@
     <xf numFmtId="0" fontId="0" fillId="52" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="33" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2989,7 +3017,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -3459,12 +3487,12 @@
         <v>58</v>
       </c>
       <c r="K1" s="56"/>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
     </row>
     <row r="2" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
@@ -3479,12 +3507,12 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
       <c r="L2" s="39" t="s">
         <v>4</v>
       </c>
@@ -3865,12 +3893,12 @@
       <c r="C11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="88" t="s">
+      <c r="L11" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
+      <c r="M11" s="107"/>
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
     </row>
     <row r="12" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
@@ -3885,12 +3913,12 @@
       <c r="E12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="89" t="s">
+      <c r="G12" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
       <c r="L12" s="12" t="s">
         <v>4</v>
       </c>
@@ -3903,12 +3931,12 @@
       <c r="O12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="89" t="s">
+      <c r="Q12" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="R12" s="89"/>
-      <c r="S12" s="89"/>
-      <c r="T12" s="89"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
     </row>
     <row r="13" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
@@ -4325,12 +4353,12 @@
       <c r="C23" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L23" s="88" t="s">
+      <c r="L23" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="107"/>
+      <c r="O23" s="107"/>
     </row>
     <row r="24" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
@@ -4345,12 +4373,12 @@
       <c r="E24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="89" t="s">
+      <c r="G24" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="89"/>
-      <c r="I24" s="89"/>
-      <c r="J24" s="89"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
       <c r="L24" s="12" t="s">
         <v>4</v>
       </c>
@@ -4363,12 +4391,12 @@
       <c r="O24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="95" t="s">
+      <c r="Q24" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="R24" s="95"/>
-      <c r="S24" s="95"/>
-      <c r="T24" s="95"/>
+      <c r="R24" s="122"/>
+      <c r="S24" s="122"/>
+      <c r="T24" s="122"/>
     </row>
     <row r="25" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
@@ -4554,12 +4582,12 @@
       <c r="C33" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L33" s="88" t="s">
+      <c r="L33" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="M33" s="88"/>
-      <c r="N33" s="88"/>
-      <c r="O33" s="88"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="107"/>
+      <c r="O33" s="107"/>
     </row>
     <row r="34" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
@@ -4574,12 +4602,12 @@
       <c r="E34" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="89" t="s">
+      <c r="G34" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="H34" s="89"/>
-      <c r="I34" s="89"/>
-      <c r="J34" s="89"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
       <c r="L34" s="12" t="s">
         <v>4</v>
       </c>
@@ -4592,12 +4620,12 @@
       <c r="O34" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="95" t="s">
+      <c r="Q34" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="R34" s="95"/>
-      <c r="S34" s="95"/>
-      <c r="T34" s="95"/>
+      <c r="R34" s="122"/>
+      <c r="S34" s="122"/>
+      <c r="T34" s="122"/>
     </row>
     <row r="35" spans="2:20" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="29" t="s">
@@ -4612,22 +4640,22 @@
       <c r="E35" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="96" t="s">
+      <c r="G35" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="97"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="98"/>
-      <c r="L35" s="92" t="s">
+      <c r="H35" s="111"/>
+      <c r="I35" s="111"/>
+      <c r="J35" s="112"/>
+      <c r="L35" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="M35" s="92" t="s">
+      <c r="M35" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="N35" s="92" t="s">
+      <c r="N35" s="119" t="s">
         <v>89</v>
       </c>
-      <c r="O35" s="92" t="s">
+      <c r="O35" s="119" t="s">
         <v>90</v>
       </c>
       <c r="Q35" s="78" t="s">
@@ -4656,14 +4684,14 @@
       <c r="E36" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="99"/>
-      <c r="H36" s="100"/>
-      <c r="I36" s="100"/>
-      <c r="J36" s="101"/>
-      <c r="L36" s="93"/>
-      <c r="M36" s="93"/>
-      <c r="N36" s="93"/>
-      <c r="O36" s="93"/>
+      <c r="G36" s="113"/>
+      <c r="H36" s="114"/>
+      <c r="I36" s="114"/>
+      <c r="J36" s="115"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="120"/>
+      <c r="N36" s="120"/>
+      <c r="O36" s="120"/>
       <c r="Q36" s="78" t="s">
         <v>92</v>
       </c>
@@ -4693,17 +4721,17 @@
       <c r="F37" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="G37" s="99"/>
-      <c r="H37" s="100"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="101"/>
+      <c r="G37" s="113"/>
+      <c r="H37" s="114"/>
+      <c r="I37" s="114"/>
+      <c r="J37" s="115"/>
       <c r="K37" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="93"/>
-      <c r="M37" s="93"/>
-      <c r="N37" s="93"/>
-      <c r="O37" s="93"/>
+      <c r="L37" s="120"/>
+      <c r="M37" s="120"/>
+      <c r="N37" s="120"/>
+      <c r="O37" s="120"/>
       <c r="P37" s="26" t="s">
         <v>60</v>
       </c>
@@ -4733,14 +4761,14 @@
       <c r="E38" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="G38" s="99"/>
-      <c r="H38" s="100"/>
-      <c r="I38" s="100"/>
-      <c r="J38" s="101"/>
-      <c r="L38" s="93"/>
-      <c r="M38" s="93"/>
-      <c r="N38" s="93"/>
-      <c r="O38" s="93"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="114"/>
+      <c r="I38" s="114"/>
+      <c r="J38" s="115"/>
+      <c r="L38" s="120"/>
+      <c r="M38" s="120"/>
+      <c r="N38" s="120"/>
+      <c r="O38" s="120"/>
       <c r="Q38" s="78" t="s">
         <v>95</v>
       </c>
@@ -4767,14 +4795,14 @@
       <c r="E39" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="99"/>
-      <c r="H39" s="100"/>
-      <c r="I39" s="100"/>
-      <c r="J39" s="101"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
-      <c r="N39" s="93"/>
-      <c r="O39" s="93"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="114"/>
+      <c r="I39" s="114"/>
+      <c r="J39" s="115"/>
+      <c r="L39" s="120"/>
+      <c r="M39" s="120"/>
+      <c r="N39" s="120"/>
+      <c r="O39" s="120"/>
       <c r="Q39" s="78" t="s">
         <v>96</v>
       </c>
@@ -4801,14 +4829,14 @@
       <c r="E40" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="102"/>
-      <c r="H40" s="103"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="104"/>
-      <c r="L40" s="94"/>
-      <c r="M40" s="94"/>
-      <c r="N40" s="94"/>
-      <c r="O40" s="94"/>
+      <c r="G40" s="116"/>
+      <c r="H40" s="117"/>
+      <c r="I40" s="117"/>
+      <c r="J40" s="118"/>
+      <c r="L40" s="121"/>
+      <c r="M40" s="121"/>
+      <c r="N40" s="121"/>
+      <c r="O40" s="121"/>
       <c r="Q40" s="78" t="s">
         <v>97</v>
       </c>
@@ -4826,12 +4854,12 @@
       <c r="C44" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="L44" s="88" t="s">
+      <c r="L44" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="M44" s="88"/>
-      <c r="N44" s="88"/>
-      <c r="O44" s="88"/>
+      <c r="M44" s="107"/>
+      <c r="N44" s="107"/>
+      <c r="O44" s="107"/>
     </row>
     <row r="45" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
@@ -4846,12 +4874,12 @@
       <c r="E45" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G45" s="89" t="s">
+      <c r="G45" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
+      <c r="H45" s="109"/>
+      <c r="I45" s="109"/>
+      <c r="J45" s="109"/>
       <c r="L45" s="12" t="s">
         <v>4</v>
       </c>
@@ -4864,26 +4892,26 @@
       <c r="O45" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q45" s="89" t="s">
+      <c r="Q45" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="R45" s="89"/>
-      <c r="S45" s="89"/>
-      <c r="T45" s="89"/>
+      <c r="R45" s="109"/>
+      <c r="S45" s="109"/>
+      <c r="T45" s="109"/>
     </row>
     <row r="46" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="50"/>
       <c r="C46" s="50"/>
       <c r="D46" s="50"/>
       <c r="E46" s="50"/>
-      <c r="G46" s="96"/>
-      <c r="H46" s="97"/>
-      <c r="I46" s="97"/>
-      <c r="J46" s="98"/>
-      <c r="L46" s="92"/>
-      <c r="M46" s="92"/>
-      <c r="N46" s="92"/>
-      <c r="O46" s="92"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="111"/>
+      <c r="I46" s="111"/>
+      <c r="J46" s="112"/>
+      <c r="L46" s="119"/>
+      <c r="M46" s="119"/>
+      <c r="N46" s="119"/>
+      <c r="O46" s="119"/>
       <c r="Q46" s="50"/>
       <c r="R46" s="50"/>
       <c r="S46" s="50"/>
@@ -4894,14 +4922,14 @@
       <c r="C47" s="50"/>
       <c r="D47" s="50"/>
       <c r="E47" s="50"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="100"/>
-      <c r="J47" s="101"/>
-      <c r="L47" s="93"/>
-      <c r="M47" s="93"/>
-      <c r="N47" s="93"/>
-      <c r="O47" s="93"/>
+      <c r="G47" s="113"/>
+      <c r="H47" s="114"/>
+      <c r="I47" s="114"/>
+      <c r="J47" s="115"/>
+      <c r="L47" s="120"/>
+      <c r="M47" s="120"/>
+      <c r="N47" s="120"/>
+      <c r="O47" s="120"/>
       <c r="Q47" s="50"/>
       <c r="R47" s="50"/>
       <c r="S47" s="50"/>
@@ -4915,17 +4943,17 @@
       <c r="F48" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="G48" s="99"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="101"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="114"/>
+      <c r="I48" s="114"/>
+      <c r="J48" s="115"/>
       <c r="K48" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="L48" s="93"/>
-      <c r="M48" s="93"/>
-      <c r="N48" s="93"/>
-      <c r="O48" s="93"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="120"/>
       <c r="P48" s="26" t="s">
         <v>60</v>
       </c>
@@ -4939,14 +4967,14 @@
       <c r="C49" s="50"/>
       <c r="D49" s="50"/>
       <c r="E49" s="50"/>
-      <c r="G49" s="99"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="101"/>
-      <c r="L49" s="93"/>
-      <c r="M49" s="93"/>
-      <c r="N49" s="93"/>
-      <c r="O49" s="93"/>
+      <c r="G49" s="113"/>
+      <c r="H49" s="114"/>
+      <c r="I49" s="114"/>
+      <c r="J49" s="115"/>
+      <c r="L49" s="120"/>
+      <c r="M49" s="120"/>
+      <c r="N49" s="120"/>
+      <c r="O49" s="120"/>
       <c r="Q49" s="50"/>
       <c r="R49" s="50"/>
       <c r="S49" s="50"/>
@@ -4957,14 +4985,14 @@
       <c r="C50" s="50"/>
       <c r="D50" s="50"/>
       <c r="E50" s="50"/>
-      <c r="G50" s="99"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="100"/>
-      <c r="J50" s="101"/>
-      <c r="L50" s="93"/>
-      <c r="M50" s="93"/>
-      <c r="N50" s="93"/>
-      <c r="O50" s="93"/>
+      <c r="G50" s="113"/>
+      <c r="H50" s="114"/>
+      <c r="I50" s="114"/>
+      <c r="J50" s="115"/>
+      <c r="L50" s="120"/>
+      <c r="M50" s="120"/>
+      <c r="N50" s="120"/>
+      <c r="O50" s="120"/>
       <c r="Q50" s="50"/>
       <c r="R50" s="50"/>
       <c r="S50" s="50"/>
@@ -4975,53 +5003,53 @@
       <c r="C51" s="50"/>
       <c r="D51" s="50"/>
       <c r="E51" s="50"/>
-      <c r="G51" s="102"/>
-      <c r="H51" s="103"/>
-      <c r="I51" s="103"/>
-      <c r="J51" s="104"/>
-      <c r="L51" s="94"/>
-      <c r="M51" s="94"/>
-      <c r="N51" s="94"/>
-      <c r="O51" s="94"/>
+      <c r="G51" s="116"/>
+      <c r="H51" s="117"/>
+      <c r="I51" s="117"/>
+      <c r="J51" s="118"/>
+      <c r="L51" s="121"/>
+      <c r="M51" s="121"/>
+      <c r="N51" s="121"/>
+      <c r="O51" s="121"/>
       <c r="Q51" s="50"/>
       <c r="R51" s="50"/>
       <c r="S51" s="50"/>
       <c r="T51" s="50"/>
     </row>
     <row r="53" spans="1:20" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B53" s="87" t="s">
+      <c r="B53" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="87"/>
-      <c r="D53" s="87"/>
-      <c r="E53" s="87"/>
+      <c r="C53" s="108"/>
+      <c r="D53" s="108"/>
+      <c r="E53" s="108"/>
       <c r="F53" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="87" t="s">
+      <c r="G53" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="H53" s="87"/>
-      <c r="I53" s="87"/>
-      <c r="J53" s="87"/>
+      <c r="H53" s="108"/>
+      <c r="I53" s="108"/>
+      <c r="J53" s="108"/>
       <c r="K53" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L53" s="87" t="s">
+      <c r="L53" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="M53" s="87"/>
-      <c r="N53" s="87"/>
-      <c r="O53" s="87"/>
+      <c r="M53" s="108"/>
+      <c r="N53" s="108"/>
+      <c r="O53" s="108"/>
       <c r="P53" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q53" s="87" t="s">
+      <c r="Q53" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="R53" s="87"/>
-      <c r="S53" s="87"/>
-      <c r="T53" s="87"/>
+      <c r="R53" s="108"/>
+      <c r="S53" s="108"/>
+      <c r="T53" s="108"/>
     </row>
     <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="39"/>
@@ -5030,24 +5058,24 @@
       </c>
       <c r="D59" s="39"/>
       <c r="E59" s="39"/>
-      <c r="G59" s="89" t="s">
+      <c r="G59" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="H59" s="89"/>
-      <c r="I59" s="89"/>
-      <c r="J59" s="89"/>
-      <c r="L59" s="88" t="s">
+      <c r="H59" s="109"/>
+      <c r="I59" s="109"/>
+      <c r="J59" s="109"/>
+      <c r="L59" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="M59" s="88"/>
-      <c r="N59" s="88"/>
-      <c r="O59" s="88"/>
-      <c r="Q59" s="89" t="s">
+      <c r="M59" s="107"/>
+      <c r="N59" s="107"/>
+      <c r="O59" s="107"/>
+      <c r="Q59" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="R59" s="89"/>
-      <c r="S59" s="89"/>
-      <c r="T59" s="89"/>
+      <c r="R59" s="109"/>
+      <c r="S59" s="109"/>
+      <c r="T59" s="109"/>
     </row>
     <row r="60" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="37"/>
@@ -5056,15 +5084,15 @@
       <c r="D60" s="50"/>
       <c r="E60" s="50"/>
       <c r="F60" s="42"/>
-      <c r="G60" s="90"/>
-      <c r="H60" s="91"/>
-      <c r="I60" s="91"/>
-      <c r="J60" s="91"/>
+      <c r="G60" s="123"/>
+      <c r="H60" s="124"/>
+      <c r="I60" s="124"/>
+      <c r="J60" s="124"/>
       <c r="K60" s="42"/>
-      <c r="L60" s="92"/>
-      <c r="M60" s="92"/>
-      <c r="N60" s="92"/>
-      <c r="O60" s="92"/>
+      <c r="L60" s="119"/>
+      <c r="M60" s="119"/>
+      <c r="N60" s="119"/>
+      <c r="O60" s="119"/>
       <c r="Q60" s="50"/>
       <c r="R60" s="50"/>
       <c r="S60" s="50"/>
@@ -5077,15 +5105,15 @@
       <c r="D61" s="50"/>
       <c r="E61" s="50"/>
       <c r="F61" s="42"/>
-      <c r="G61" s="91"/>
-      <c r="H61" s="91"/>
-      <c r="I61" s="91"/>
-      <c r="J61" s="91"/>
+      <c r="G61" s="124"/>
+      <c r="H61" s="124"/>
+      <c r="I61" s="124"/>
+      <c r="J61" s="124"/>
       <c r="K61" s="42"/>
-      <c r="L61" s="93"/>
-      <c r="M61" s="93"/>
-      <c r="N61" s="93"/>
-      <c r="O61" s="93"/>
+      <c r="L61" s="120"/>
+      <c r="M61" s="120"/>
+      <c r="N61" s="120"/>
+      <c r="O61" s="120"/>
       <c r="Q61" s="50"/>
       <c r="R61" s="50"/>
       <c r="S61" s="50"/>
@@ -5100,17 +5128,17 @@
       <c r="F62" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="G62" s="91"/>
-      <c r="H62" s="91"/>
-      <c r="I62" s="91"/>
-      <c r="J62" s="91"/>
+      <c r="G62" s="124"/>
+      <c r="H62" s="124"/>
+      <c r="I62" s="124"/>
+      <c r="J62" s="124"/>
       <c r="K62" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="L62" s="93"/>
-      <c r="M62" s="93"/>
-      <c r="N62" s="93"/>
-      <c r="O62" s="93"/>
+      <c r="L62" s="120"/>
+      <c r="M62" s="120"/>
+      <c r="N62" s="120"/>
+      <c r="O62" s="120"/>
       <c r="P62" s="26" t="s">
         <v>60</v>
       </c>
@@ -5126,14 +5154,14 @@
       <c r="D63" s="50"/>
       <c r="E63" s="50"/>
       <c r="F63" s="42"/>
-      <c r="G63" s="91"/>
-      <c r="H63" s="91"/>
-      <c r="I63" s="91"/>
-      <c r="J63" s="91"/>
-      <c r="L63" s="93"/>
-      <c r="M63" s="93"/>
-      <c r="N63" s="93"/>
-      <c r="O63" s="93"/>
+      <c r="G63" s="124"/>
+      <c r="H63" s="124"/>
+      <c r="I63" s="124"/>
+      <c r="J63" s="124"/>
+      <c r="L63" s="120"/>
+      <c r="M63" s="120"/>
+      <c r="N63" s="120"/>
+      <c r="O63" s="120"/>
       <c r="Q63" s="50"/>
       <c r="R63" s="50"/>
       <c r="S63" s="50"/>
@@ -5146,14 +5174,14 @@
       <c r="D64" s="50"/>
       <c r="E64" s="50"/>
       <c r="F64" s="42"/>
-      <c r="G64" s="91"/>
-      <c r="H64" s="91"/>
-      <c r="I64" s="91"/>
-      <c r="J64" s="91"/>
-      <c r="L64" s="93"/>
-      <c r="M64" s="93"/>
-      <c r="N64" s="93"/>
-      <c r="O64" s="93"/>
+      <c r="G64" s="124"/>
+      <c r="H64" s="124"/>
+      <c r="I64" s="124"/>
+      <c r="J64" s="124"/>
+      <c r="L64" s="120"/>
+      <c r="M64" s="120"/>
+      <c r="N64" s="120"/>
+      <c r="O64" s="120"/>
       <c r="Q64" s="50"/>
       <c r="R64" s="50"/>
       <c r="S64" s="50"/>
@@ -5166,14 +5194,14 @@
       <c r="D65" s="50"/>
       <c r="E65" s="50"/>
       <c r="F65" s="42"/>
-      <c r="G65" s="91"/>
-      <c r="H65" s="91"/>
-      <c r="I65" s="91"/>
-      <c r="J65" s="91"/>
-      <c r="L65" s="94"/>
-      <c r="M65" s="94"/>
-      <c r="N65" s="94"/>
-      <c r="O65" s="94"/>
+      <c r="G65" s="124"/>
+      <c r="H65" s="124"/>
+      <c r="I65" s="124"/>
+      <c r="J65" s="124"/>
+      <c r="L65" s="121"/>
+      <c r="M65" s="121"/>
+      <c r="N65" s="121"/>
+      <c r="O65" s="121"/>
       <c r="Q65" s="50"/>
       <c r="R65" s="50"/>
       <c r="S65" s="50"/>
@@ -5186,42 +5214,66 @@
       <c r="J66" s="56"/>
     </row>
     <row r="67" spans="1:20" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B67" s="87" t="s">
+      <c r="B67" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="87"/>
-      <c r="D67" s="87"/>
-      <c r="E67" s="87"/>
+      <c r="C67" s="108"/>
+      <c r="D67" s="108"/>
+      <c r="E67" s="108"/>
       <c r="F67" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G67" s="87" t="s">
+      <c r="G67" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="H67" s="87"/>
-      <c r="I67" s="87"/>
-      <c r="J67" s="87"/>
+      <c r="H67" s="108"/>
+      <c r="I67" s="108"/>
+      <c r="J67" s="108"/>
       <c r="K67" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="L67" s="87" t="s">
+      <c r="L67" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="M67" s="87"/>
-      <c r="N67" s="87"/>
-      <c r="O67" s="87"/>
+      <c r="M67" s="108"/>
+      <c r="N67" s="108"/>
+      <c r="O67" s="108"/>
       <c r="P67" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Q67" s="87" t="s">
+      <c r="Q67" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="R67" s="87"/>
-      <c r="S67" s="87"/>
-      <c r="T67" s="87"/>
+      <c r="R67" s="108"/>
+      <c r="S67" s="108"/>
+      <c r="T67" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="L67:O67"/>
+    <mergeCell ref="Q67:T67"/>
+    <mergeCell ref="L59:O59"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="Q59:T59"/>
+    <mergeCell ref="G60:J65"/>
+    <mergeCell ref="L60:L65"/>
+    <mergeCell ref="M60:M65"/>
+    <mergeCell ref="N60:N65"/>
+    <mergeCell ref="O60:O65"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="Q34:T34"/>
+    <mergeCell ref="G35:J40"/>
+    <mergeCell ref="L35:L40"/>
+    <mergeCell ref="M35:M40"/>
+    <mergeCell ref="N35:N40"/>
+    <mergeCell ref="O35:O40"/>
+    <mergeCell ref="Q24:T24"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="L33:O33"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="G53:J53"/>
@@ -5238,30 +5290,6 @@
     <mergeCell ref="O46:O51"/>
     <mergeCell ref="L23:O23"/>
     <mergeCell ref="G24:J24"/>
-    <mergeCell ref="Q24:T24"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="Q12:T12"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="Q34:T34"/>
-    <mergeCell ref="G35:J40"/>
-    <mergeCell ref="L35:L40"/>
-    <mergeCell ref="M35:M40"/>
-    <mergeCell ref="N35:N40"/>
-    <mergeCell ref="O35:O40"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="G67:J67"/>
-    <mergeCell ref="L67:O67"/>
-    <mergeCell ref="Q67:T67"/>
-    <mergeCell ref="L59:O59"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="Q59:T59"/>
-    <mergeCell ref="G60:J65"/>
-    <mergeCell ref="L60:L65"/>
-    <mergeCell ref="M60:M65"/>
-    <mergeCell ref="N60:N65"/>
-    <mergeCell ref="O60:O65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5719,8 +5747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D94007A-DED6-4AF2-97A7-B116AC4456BC}">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5738,18 +5766,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="87" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="87" t="s">
         <v>159</v>
       </c>
       <c r="D2" s="71">
@@ -6046,55 +6074,45 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="107" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D18" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
-      <c r="I18" s="107" t="s">
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="125"/>
+      <c r="I18" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="J18" s="107"/>
-      <c r="K18" s="107"/>
-      <c r="L18" s="107"/>
-      <c r="N18" s="107" t="s">
+      <c r="J18" s="125"/>
+      <c r="K18" s="125"/>
+      <c r="L18" s="125"/>
+      <c r="N18" s="125" t="s">
         <v>163</v>
       </c>
-      <c r="O18" s="107"/>
-      <c r="P18" s="107"/>
-      <c r="Q18" s="107"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E19" s="130" t="s">
+      <c r="O18" s="125"/>
+      <c r="P18" s="125"/>
+      <c r="Q18" s="125"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F19" s="130"/>
-      <c r="G19" s="130"/>
-      <c r="H19" s="130"/>
-      <c r="I19" s="130"/>
-      <c r="J19" s="130" t="s">
+      <c r="J19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K19" s="130"/>
-      <c r="L19" s="130"/>
-      <c r="N19" s="130"/>
-      <c r="O19" s="130" t="s">
+      <c r="O19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="P19" s="130"/>
-      <c r="Q19" s="130"/>
-      <c r="R19" s="130"/>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="110" t="s">
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="B20" s="110" t="s">
+      <c r="B20" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="C20" s="110" t="s">
+      <c r="C20" s="87" t="s">
         <v>163</v>
       </c>
       <c r="D20" s="71">
@@ -6134,7 +6152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>161</v>
       </c>
@@ -6168,20 +6186,20 @@
       <c r="L21" s="46">
         <v>50</v>
       </c>
-      <c r="N21" s="112">
+      <c r="N21" s="89">
         <v>47</v>
       </c>
-      <c r="O21" s="112">
+      <c r="O21" s="89">
         <v>49</v>
       </c>
-      <c r="P21" s="112">
+      <c r="P21" s="89">
         <v>56</v>
       </c>
-      <c r="Q21" s="112">
+      <c r="Q21" s="89">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>161</v>
       </c>
@@ -6228,7 +6246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>161</v>
       </c>
@@ -6262,20 +6280,20 @@
       <c r="L23" s="46">
         <v>94</v>
       </c>
-      <c r="N23" s="113">
+      <c r="N23" s="90">
         <v>90</v>
       </c>
-      <c r="O23" s="113">
+      <c r="O23" s="90">
         <v>94</v>
       </c>
-      <c r="P23" s="113">
+      <c r="P23" s="90">
         <v>85</v>
       </c>
-      <c r="Q23" s="113">
+      <c r="Q23" s="90">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
@@ -6297,32 +6315,32 @@
       <c r="G24" s="46">
         <v>72</v>
       </c>
-      <c r="I24" s="114">
+      <c r="I24" s="91">
         <v>63</v>
       </c>
-      <c r="J24" s="114">
+      <c r="J24" s="91">
         <v>68</v>
       </c>
-      <c r="K24" s="114">
+      <c r="K24" s="91">
         <v>64</v>
       </c>
-      <c r="L24" s="114">
+      <c r="L24" s="91">
         <v>72</v>
       </c>
-      <c r="N24" s="112">
+      <c r="N24" s="89">
         <v>63</v>
       </c>
-      <c r="O24" s="112">
+      <c r="O24" s="89">
         <v>68</v>
       </c>
-      <c r="P24" s="112">
+      <c r="P24" s="89">
         <v>64</v>
       </c>
-      <c r="Q24" s="112">
+      <c r="Q24" s="89">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>161</v>
       </c>
@@ -6344,16 +6362,16 @@
       <c r="G25" s="46">
         <v>62</v>
       </c>
-      <c r="I25" s="114">
+      <c r="I25" s="91">
         <v>73</v>
       </c>
-      <c r="J25" s="114">
+      <c r="J25" s="91">
         <v>70</v>
       </c>
-      <c r="K25" s="114">
+      <c r="K25" s="91">
         <v>67</v>
       </c>
-      <c r="L25" s="114">
+      <c r="L25" s="91">
         <v>62</v>
       </c>
       <c r="N25" s="46">
@@ -6369,7 +6387,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>161</v>
       </c>
@@ -6391,32 +6409,32 @@
       <c r="G26" s="46">
         <v>66</v>
       </c>
-      <c r="I26" s="114">
+      <c r="I26" s="91">
         <v>68</v>
       </c>
-      <c r="J26" s="114">
+      <c r="J26" s="91">
         <v>75</v>
       </c>
-      <c r="K26" s="114">
+      <c r="K26" s="91">
         <v>58</v>
       </c>
-      <c r="L26" s="114">
+      <c r="L26" s="91">
         <v>66</v>
       </c>
-      <c r="N26" s="113">
+      <c r="N26" s="90">
         <v>68</v>
       </c>
-      <c r="O26" s="113">
+      <c r="O26" s="90">
         <v>75</v>
       </c>
-      <c r="P26" s="113">
+      <c r="P26" s="90">
         <v>58</v>
       </c>
-      <c r="Q26" s="113">
+      <c r="Q26" s="90">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>160</v>
       </c>
@@ -6426,16 +6444,16 @@
       <c r="C27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="111">
+      <c r="D27" s="88">
         <v>76</v>
       </c>
-      <c r="E27" s="111">
+      <c r="E27" s="88">
         <v>90</v>
       </c>
-      <c r="F27" s="111">
+      <c r="F27" s="88">
         <v>89</v>
       </c>
-      <c r="G27" s="111">
+      <c r="G27" s="88">
         <v>93</v>
       </c>
       <c r="I27" s="46">
@@ -6450,20 +6468,20 @@
       <c r="L27" s="46">
         <v>93</v>
       </c>
-      <c r="N27" s="112">
+      <c r="N27" s="89">
         <v>76</v>
       </c>
-      <c r="O27" s="112">
+      <c r="O27" s="89">
         <v>90</v>
       </c>
-      <c r="P27" s="112">
+      <c r="P27" s="89">
         <v>89</v>
       </c>
-      <c r="Q27" s="112">
+      <c r="Q27" s="89">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>160</v>
       </c>
@@ -6473,16 +6491,16 @@
       <c r="C28" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D28" s="111">
+      <c r="D28" s="88">
         <v>68</v>
       </c>
-      <c r="E28" s="111">
+      <c r="E28" s="88">
         <v>71</v>
       </c>
-      <c r="F28" s="111">
+      <c r="F28" s="88">
         <v>78</v>
       </c>
-      <c r="G28" s="111">
+      <c r="G28" s="88">
         <v>65</v>
       </c>
       <c r="I28" s="46">
@@ -6510,7 +6528,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>160</v>
       </c>
@@ -6520,16 +6538,16 @@
       <c r="C29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D29" s="111">
+      <c r="D29" s="88">
         <v>46</v>
       </c>
-      <c r="E29" s="111">
+      <c r="E29" s="88">
         <v>52</v>
       </c>
-      <c r="F29" s="111">
+      <c r="F29" s="88">
         <v>58</v>
       </c>
-      <c r="G29" s="111">
+      <c r="G29" s="88">
         <v>48</v>
       </c>
       <c r="I29" s="46">
@@ -6544,20 +6562,20 @@
       <c r="L29" s="46">
         <v>48</v>
       </c>
-      <c r="N29" s="113">
+      <c r="N29" s="90">
         <v>46</v>
       </c>
-      <c r="O29" s="113">
+      <c r="O29" s="90">
         <v>52</v>
       </c>
-      <c r="P29" s="113">
+      <c r="P29" s="90">
         <v>58</v>
       </c>
-      <c r="Q29" s="113">
+      <c r="Q29" s="90">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>160</v>
       </c>
@@ -6567,44 +6585,44 @@
       <c r="C30" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="111">
+      <c r="D30" s="88">
         <v>86</v>
       </c>
-      <c r="E30" s="111">
+      <c r="E30" s="88">
         <v>77</v>
       </c>
-      <c r="F30" s="111">
+      <c r="F30" s="88">
         <v>79</v>
       </c>
-      <c r="G30" s="111">
+      <c r="G30" s="88">
         <v>75</v>
       </c>
-      <c r="I30" s="114">
+      <c r="I30" s="91">
         <v>86</v>
       </c>
-      <c r="J30" s="114">
+      <c r="J30" s="91">
         <v>77</v>
       </c>
-      <c r="K30" s="114">
+      <c r="K30" s="91">
         <v>79</v>
       </c>
-      <c r="L30" s="114">
+      <c r="L30" s="91">
         <v>75</v>
       </c>
-      <c r="N30" s="112">
+      <c r="N30" s="89">
         <v>86</v>
       </c>
-      <c r="O30" s="112">
+      <c r="O30" s="89">
         <v>77</v>
       </c>
-      <c r="P30" s="112">
+      <c r="P30" s="89">
         <v>79</v>
       </c>
-      <c r="Q30" s="112">
+      <c r="Q30" s="89">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -6614,28 +6632,28 @@
       <c r="C31" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D31" s="111">
+      <c r="D31" s="88">
         <v>79</v>
       </c>
-      <c r="E31" s="111">
+      <c r="E31" s="88">
         <v>62</v>
       </c>
-      <c r="F31" s="111">
+      <c r="F31" s="88">
         <v>67</v>
       </c>
-      <c r="G31" s="111">
+      <c r="G31" s="88">
         <v>70</v>
       </c>
-      <c r="I31" s="114">
+      <c r="I31" s="91">
         <v>79</v>
       </c>
-      <c r="J31" s="114">
+      <c r="J31" s="91">
         <v>62</v>
       </c>
-      <c r="K31" s="114">
+      <c r="K31" s="91">
         <v>67</v>
       </c>
-      <c r="L31" s="114">
+      <c r="L31" s="91">
         <v>70</v>
       </c>
       <c r="N31" s="46">
@@ -6651,7 +6669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>160</v>
       </c>
@@ -6661,40 +6679,40 @@
       <c r="C32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D32" s="111">
+      <c r="D32" s="88">
         <v>57</v>
       </c>
-      <c r="E32" s="111">
+      <c r="E32" s="88">
         <v>67</v>
       </c>
-      <c r="F32" s="111">
+      <c r="F32" s="88">
         <v>53</v>
       </c>
-      <c r="G32" s="111">
+      <c r="G32" s="88">
         <v>66</v>
       </c>
-      <c r="I32" s="114">
+      <c r="I32" s="91">
         <v>57</v>
       </c>
-      <c r="J32" s="114">
+      <c r="J32" s="91">
         <v>67</v>
       </c>
-      <c r="K32" s="114">
+      <c r="K32" s="91">
         <v>53</v>
       </c>
-      <c r="L32" s="114">
+      <c r="L32" s="91">
         <v>66</v>
       </c>
-      <c r="N32" s="113">
+      <c r="N32" s="90">
         <v>57</v>
       </c>
-      <c r="O32" s="113">
+      <c r="O32" s="90">
         <v>67</v>
       </c>
-      <c r="P32" s="113">
+      <c r="P32" s="90">
         <v>53</v>
       </c>
-      <c r="Q32" s="113">
+      <c r="Q32" s="90">
         <v>66</v>
       </c>
     </row>
@@ -6704,81 +6722,63 @@
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="T35" s="110" t="s">
+      <c r="T35" s="87" t="s">
         <v>169</v>
       </c>
-      <c r="U35" s="110"/>
-      <c r="V35" s="110"/>
+      <c r="U35" s="87"/>
+      <c r="V35" s="87"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E36" s="110" t="s">
+      <c r="E36" s="87" t="s">
         <v>168</v>
       </c>
-      <c r="F36" s="110"/>
-      <c r="G36" s="110"/>
-      <c r="H36" s="110"/>
-      <c r="I36" s="110"/>
-      <c r="J36" s="110" t="s">
+      <c r="F36" s="87"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="87"/>
+      <c r="I36" s="87"/>
+      <c r="J36" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="K36" s="110"/>
-      <c r="L36" s="110"/>
-      <c r="M36" s="110"/>
-      <c r="N36" s="110"/>
-      <c r="O36" s="110" t="s">
+      <c r="K36" s="87"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="87"/>
+      <c r="O36" s="87" t="s">
         <v>171</v>
       </c>
-      <c r="P36" s="110"/>
-      <c r="Q36" s="110"/>
-      <c r="R36" s="110"/>
-      <c r="S36" s="110"/>
-      <c r="W36" s="107" t="s">
+      <c r="P36" s="87"/>
+      <c r="Q36" s="87"/>
+      <c r="R36" s="87"/>
+      <c r="S36" s="87"/>
+      <c r="W36" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="X36" s="107"/>
-      <c r="Y36" s="107"/>
-      <c r="Z36" s="107"/>
+      <c r="X36" s="125"/>
+      <c r="Y36" s="125"/>
+      <c r="Z36" s="125"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E37" s="130" t="s">
+      <c r="E37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F37" s="130"/>
-      <c r="G37" s="130"/>
-      <c r="H37" s="130"/>
-      <c r="I37" s="130"/>
-      <c r="J37" s="130" t="s">
+      <c r="J37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K37" s="130"/>
-      <c r="L37" s="130"/>
-      <c r="M37" s="130"/>
-      <c r="N37" s="130"/>
-      <c r="O37" s="130" t="s">
+      <c r="O37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="P37" s="130"/>
-      <c r="Q37" s="130"/>
-      <c r="R37" s="130"/>
-      <c r="S37" s="130"/>
-      <c r="T37" s="130"/>
-      <c r="U37" s="130"/>
-      <c r="V37" s="130"/>
-      <c r="W37" s="130"/>
-      <c r="X37" s="130" t="s">
+      <c r="X37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="Y37" s="130"/>
-      <c r="Z37" s="130"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="110" t="s">
+      <c r="A38" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="110" t="s">
+      <c r="B38" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="C38" s="110" t="s">
+      <c r="C38" s="87" t="s">
         <v>163</v>
       </c>
       <c r="D38" s="71">
@@ -6817,13 +6817,13 @@
       <c r="Q38" s="71">
         <v>4</v>
       </c>
-      <c r="T38" s="110" t="s">
+      <c r="T38" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="U38" s="110" t="s">
+      <c r="U38" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="V38" s="110" t="s">
+      <c r="V38" s="87" t="s">
         <v>163</v>
       </c>
       <c r="W38" s="71">
@@ -6849,40 +6849,40 @@
       <c r="C39" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="117">
+      <c r="D39" s="94">
         <v>47</v>
       </c>
-      <c r="E39" s="117">
+      <c r="E39" s="94">
         <v>49</v>
       </c>
-      <c r="F39" s="117">
+      <c r="F39" s="94">
         <v>56</v>
       </c>
-      <c r="G39" s="117">
+      <c r="G39" s="94">
         <v>50</v>
       </c>
-      <c r="I39" s="118">
+      <c r="I39" s="95">
         <v>86</v>
       </c>
-      <c r="J39" s="118">
+      <c r="J39" s="95">
         <v>77</v>
       </c>
-      <c r="K39" s="118">
+      <c r="K39" s="95">
         <v>79</v>
       </c>
-      <c r="L39" s="118">
+      <c r="L39" s="95">
         <v>75</v>
       </c>
-      <c r="N39" s="115">
+      <c r="N39" s="92">
         <v>47</v>
       </c>
-      <c r="O39" s="115">
+      <c r="O39" s="92">
         <v>49</v>
       </c>
-      <c r="P39" s="115">
+      <c r="P39" s="92">
         <v>56</v>
       </c>
-      <c r="Q39" s="115">
+      <c r="Q39" s="92">
         <v>50</v>
       </c>
       <c r="T39" s="1" t="s">
@@ -6894,16 +6894,16 @@
       <c r="V39" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="W39" s="120">
+      <c r="W39" s="97">
         <v>86</v>
       </c>
-      <c r="X39" s="120">
+      <c r="X39" s="97">
         <v>77</v>
       </c>
-      <c r="Y39" s="120">
+      <c r="Y39" s="97">
         <v>79</v>
       </c>
-      <c r="Z39" s="120">
+      <c r="Z39" s="97">
         <v>75</v>
       </c>
     </row>
@@ -6917,40 +6917,40 @@
       <c r="C40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="117">
+      <c r="D40" s="94">
         <v>69</v>
       </c>
-      <c r="E40" s="117">
+      <c r="E40" s="94">
         <v>72</v>
       </c>
-      <c r="F40" s="117">
+      <c r="F40" s="94">
         <v>61</v>
       </c>
-      <c r="G40" s="117">
+      <c r="G40" s="94">
         <v>74</v>
       </c>
-      <c r="I40" s="119">
+      <c r="I40" s="96">
         <v>57</v>
       </c>
-      <c r="J40" s="119">
+      <c r="J40" s="96">
         <v>67</v>
       </c>
-      <c r="K40" s="119">
+      <c r="K40" s="96">
         <v>53</v>
       </c>
-      <c r="L40" s="119">
+      <c r="L40" s="96">
         <v>66</v>
       </c>
-      <c r="N40" s="116">
+      <c r="N40" s="93">
         <v>69</v>
       </c>
-      <c r="O40" s="116">
+      <c r="O40" s="93">
         <v>72</v>
       </c>
-      <c r="P40" s="116">
+      <c r="P40" s="93">
         <v>61</v>
       </c>
-      <c r="Q40" s="116">
+      <c r="Q40" s="93">
         <v>74</v>
       </c>
       <c r="T40" s="1" t="s">
@@ -6962,16 +6962,16 @@
       <c r="V40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="W40" s="121">
+      <c r="W40" s="98">
         <v>57</v>
       </c>
-      <c r="X40" s="121">
+      <c r="X40" s="98">
         <v>67</v>
       </c>
-      <c r="Y40" s="121">
+      <c r="Y40" s="98">
         <v>53</v>
       </c>
-      <c r="Z40" s="121">
+      <c r="Z40" s="98">
         <v>66</v>
       </c>
     </row>
@@ -6985,40 +6985,40 @@
       <c r="C41" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D41" s="117">
+      <c r="D41" s="94">
         <v>90</v>
       </c>
-      <c r="E41" s="117">
+      <c r="E41" s="94">
         <v>94</v>
       </c>
-      <c r="F41" s="117">
+      <c r="F41" s="94">
         <v>85</v>
       </c>
-      <c r="G41" s="117">
+      <c r="G41" s="94">
         <v>94</v>
       </c>
-      <c r="I41" s="114">
+      <c r="I41" s="91">
         <v>79</v>
       </c>
-      <c r="J41" s="114">
+      <c r="J41" s="91">
         <v>62</v>
       </c>
-      <c r="K41" s="114">
+      <c r="K41" s="91">
         <v>67</v>
       </c>
-      <c r="L41" s="114">
+      <c r="L41" s="91">
         <v>70</v>
       </c>
-      <c r="N41" s="111">
+      <c r="N41" s="88">
         <v>90</v>
       </c>
-      <c r="O41" s="111">
+      <c r="O41" s="88">
         <v>94</v>
       </c>
-      <c r="P41" s="111">
+      <c r="P41" s="88">
         <v>85</v>
       </c>
-      <c r="Q41" s="111">
+      <c r="Q41" s="88">
         <v>94</v>
       </c>
       <c r="T41" s="1" t="s">
@@ -7030,16 +7030,16 @@
       <c r="V41" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="W41" s="122">
+      <c r="W41" s="99">
         <v>79</v>
       </c>
-      <c r="X41" s="122">
+      <c r="X41" s="99">
         <v>62</v>
       </c>
-      <c r="Y41" s="122">
+      <c r="Y41" s="99">
         <v>67</v>
       </c>
-      <c r="Z41" s="122">
+      <c r="Z41" s="99">
         <v>70</v>
       </c>
     </row>
@@ -7053,40 +7053,40 @@
       <c r="C42" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D42" s="114">
+      <c r="D42" s="91">
         <v>63</v>
       </c>
-      <c r="E42" s="114">
+      <c r="E42" s="91">
         <v>68</v>
       </c>
-      <c r="F42" s="114">
+      <c r="F42" s="91">
         <v>64</v>
       </c>
-      <c r="G42" s="114">
+      <c r="G42" s="91">
         <v>72</v>
       </c>
-      <c r="I42" s="118">
+      <c r="I42" s="95">
         <v>63</v>
       </c>
-      <c r="J42" s="118">
+      <c r="J42" s="95">
         <v>68</v>
       </c>
-      <c r="K42" s="118">
+      <c r="K42" s="95">
         <v>64</v>
       </c>
-      <c r="L42" s="118">
+      <c r="L42" s="95">
         <v>72</v>
       </c>
-      <c r="N42" s="112">
+      <c r="N42" s="89">
         <v>63</v>
       </c>
-      <c r="O42" s="112">
+      <c r="O42" s="89">
         <v>68</v>
       </c>
-      <c r="P42" s="112">
+      <c r="P42" s="89">
         <v>64</v>
       </c>
-      <c r="Q42" s="112">
+      <c r="Q42" s="89">
         <v>72</v>
       </c>
       <c r="T42" s="1" t="s">
@@ -7098,16 +7098,16 @@
       <c r="V42" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="W42" s="123">
+      <c r="W42" s="100">
         <v>63</v>
       </c>
-      <c r="X42" s="123">
+      <c r="X42" s="100">
         <v>68</v>
       </c>
-      <c r="Y42" s="123">
+      <c r="Y42" s="100">
         <v>64</v>
       </c>
-      <c r="Z42" s="123">
+      <c r="Z42" s="100">
         <v>72</v>
       </c>
     </row>
@@ -7121,40 +7121,40 @@
       <c r="C43" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D43" s="114">
+      <c r="D43" s="91">
         <v>73</v>
       </c>
-      <c r="E43" s="114">
+      <c r="E43" s="91">
         <v>70</v>
       </c>
-      <c r="F43" s="114">
+      <c r="F43" s="91">
         <v>67</v>
       </c>
-      <c r="G43" s="114">
+      <c r="G43" s="91">
         <v>62</v>
       </c>
-      <c r="I43" s="119">
+      <c r="I43" s="96">
         <v>68</v>
       </c>
-      <c r="J43" s="119">
+      <c r="J43" s="96">
         <v>75</v>
       </c>
-      <c r="K43" s="119">
+      <c r="K43" s="96">
         <v>58</v>
       </c>
-      <c r="L43" s="119">
+      <c r="L43" s="96">
         <v>66</v>
       </c>
-      <c r="N43" s="113">
+      <c r="N43" s="90">
         <v>73</v>
       </c>
-      <c r="O43" s="113">
+      <c r="O43" s="90">
         <v>70</v>
       </c>
-      <c r="P43" s="113">
+      <c r="P43" s="90">
         <v>67</v>
       </c>
-      <c r="Q43" s="113">
+      <c r="Q43" s="90">
         <v>62</v>
       </c>
       <c r="T43" s="1" t="s">
@@ -7166,16 +7166,16 @@
       <c r="V43" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="W43" s="124">
+      <c r="W43" s="101">
         <v>68</v>
       </c>
-      <c r="X43" s="124">
+      <c r="X43" s="101">
         <v>75</v>
       </c>
-      <c r="Y43" s="124">
+      <c r="Y43" s="101">
         <v>58</v>
       </c>
-      <c r="Z43" s="124">
+      <c r="Z43" s="101">
         <v>66</v>
       </c>
     </row>
@@ -7189,28 +7189,28 @@
       <c r="C44" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D44" s="114">
+      <c r="D44" s="91">
         <v>68</v>
       </c>
-      <c r="E44" s="114">
+      <c r="E44" s="91">
         <v>75</v>
       </c>
-      <c r="F44" s="114">
+      <c r="F44" s="91">
         <v>58</v>
       </c>
-      <c r="G44" s="114">
+      <c r="G44" s="91">
         <v>66</v>
       </c>
-      <c r="I44" s="114">
+      <c r="I44" s="91">
         <v>73</v>
       </c>
-      <c r="J44" s="114">
+      <c r="J44" s="91">
         <v>70</v>
       </c>
-      <c r="K44" s="114">
+      <c r="K44" s="91">
         <v>67</v>
       </c>
-      <c r="L44" s="114">
+      <c r="L44" s="91">
         <v>62</v>
       </c>
       <c r="N44" s="46">
@@ -7257,40 +7257,40 @@
       <c r="C45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D45" s="111">
+      <c r="D45" s="88">
         <v>76</v>
       </c>
-      <c r="E45" s="111">
+      <c r="E45" s="88">
         <v>90</v>
       </c>
-      <c r="F45" s="111">
+      <c r="F45" s="88">
         <v>89</v>
       </c>
-      <c r="G45" s="111">
+      <c r="G45" s="88">
         <v>93</v>
       </c>
-      <c r="I45" s="112">
+      <c r="I45" s="89">
         <v>76</v>
       </c>
-      <c r="J45" s="112">
+      <c r="J45" s="89">
         <v>90</v>
       </c>
-      <c r="K45" s="112">
+      <c r="K45" s="89">
         <v>89</v>
       </c>
-      <c r="L45" s="112">
+      <c r="L45" s="89">
         <v>93</v>
       </c>
-      <c r="N45" s="115">
+      <c r="N45" s="92">
         <v>76</v>
       </c>
-      <c r="O45" s="115">
+      <c r="O45" s="92">
         <v>90</v>
       </c>
-      <c r="P45" s="115">
+      <c r="P45" s="92">
         <v>89</v>
       </c>
-      <c r="Q45" s="115">
+      <c r="Q45" s="92">
         <v>93</v>
       </c>
       <c r="T45" s="1" t="s">
@@ -7302,16 +7302,16 @@
       <c r="V45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="W45" s="125">
+      <c r="W45" s="102">
         <v>76</v>
       </c>
-      <c r="X45" s="125">
+      <c r="X45" s="102">
         <v>90</v>
       </c>
-      <c r="Y45" s="125">
+      <c r="Y45" s="102">
         <v>89</v>
       </c>
-      <c r="Z45" s="125">
+      <c r="Z45" s="102">
         <v>93</v>
       </c>
     </row>
@@ -7325,40 +7325,40 @@
       <c r="C46" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="111">
+      <c r="D46" s="88">
         <v>68</v>
       </c>
-      <c r="E46" s="111">
+      <c r="E46" s="88">
         <v>71</v>
       </c>
-      <c r="F46" s="111">
+      <c r="F46" s="88">
         <v>78</v>
       </c>
-      <c r="G46" s="111">
+      <c r="G46" s="88">
         <v>65</v>
       </c>
-      <c r="I46" s="113">
+      <c r="I46" s="90">
         <v>46</v>
       </c>
-      <c r="J46" s="113">
+      <c r="J46" s="90">
         <v>52</v>
       </c>
-      <c r="K46" s="113">
+      <c r="K46" s="90">
         <v>58</v>
       </c>
-      <c r="L46" s="113">
+      <c r="L46" s="90">
         <v>48</v>
       </c>
-      <c r="N46" s="116">
+      <c r="N46" s="93">
         <v>68</v>
       </c>
-      <c r="O46" s="116">
+      <c r="O46" s="93">
         <v>71</v>
       </c>
-      <c r="P46" s="116">
+      <c r="P46" s="93">
         <v>78</v>
       </c>
-      <c r="Q46" s="116">
+      <c r="Q46" s="93">
         <v>65</v>
       </c>
       <c r="T46" s="1" t="s">
@@ -7370,16 +7370,16 @@
       <c r="V46" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="W46" s="126">
+      <c r="W46" s="103">
         <v>46</v>
       </c>
-      <c r="X46" s="126">
+      <c r="X46" s="103">
         <v>52</v>
       </c>
-      <c r="Y46" s="126">
+      <c r="Y46" s="103">
         <v>58</v>
       </c>
-      <c r="Z46" s="126">
+      <c r="Z46" s="103">
         <v>48</v>
       </c>
     </row>
@@ -7393,16 +7393,16 @@
       <c r="C47" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D47" s="111">
+      <c r="D47" s="88">
         <v>46</v>
       </c>
-      <c r="E47" s="111">
+      <c r="E47" s="88">
         <v>52</v>
       </c>
-      <c r="F47" s="111">
+      <c r="F47" s="88">
         <v>58</v>
       </c>
-      <c r="G47" s="111">
+      <c r="G47" s="88">
         <v>48</v>
       </c>
       <c r="I47" s="46">
@@ -7417,16 +7417,16 @@
       <c r="L47" s="46">
         <v>65</v>
       </c>
-      <c r="N47" s="111">
+      <c r="N47" s="88">
         <v>46</v>
       </c>
-      <c r="O47" s="111">
+      <c r="O47" s="88">
         <v>52</v>
       </c>
-      <c r="P47" s="111">
+      <c r="P47" s="88">
         <v>58</v>
       </c>
-      <c r="Q47" s="111">
+      <c r="Q47" s="88">
         <v>48</v>
       </c>
       <c r="T47" s="1" t="s">
@@ -7438,16 +7438,16 @@
       <c r="V47" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="W47" s="111">
+      <c r="W47" s="88">
         <v>68</v>
       </c>
-      <c r="X47" s="111">
+      <c r="X47" s="88">
         <v>71</v>
       </c>
-      <c r="Y47" s="111">
+      <c r="Y47" s="88">
         <v>78</v>
       </c>
-      <c r="Z47" s="111">
+      <c r="Z47" s="88">
         <v>65</v>
       </c>
     </row>
@@ -7473,28 +7473,28 @@
       <c r="G48" s="46">
         <v>75</v>
       </c>
-      <c r="I48" s="112">
+      <c r="I48" s="89">
         <v>47</v>
       </c>
-      <c r="J48" s="112">
+      <c r="J48" s="89">
         <v>49</v>
       </c>
-      <c r="K48" s="112">
+      <c r="K48" s="89">
         <v>56</v>
       </c>
-      <c r="L48" s="112">
+      <c r="L48" s="89">
         <v>50</v>
       </c>
-      <c r="N48" s="112">
+      <c r="N48" s="89">
         <v>86</v>
       </c>
-      <c r="O48" s="112">
+      <c r="O48" s="89">
         <v>77</v>
       </c>
-      <c r="P48" s="112">
+      <c r="P48" s="89">
         <v>79</v>
       </c>
-      <c r="Q48" s="112">
+      <c r="Q48" s="89">
         <v>75</v>
       </c>
       <c r="T48" s="1" t="s">
@@ -7506,16 +7506,16 @@
       <c r="V48" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="W48" s="127">
+      <c r="W48" s="104">
         <v>47</v>
       </c>
-      <c r="X48" s="127">
+      <c r="X48" s="104">
         <v>49</v>
       </c>
-      <c r="Y48" s="127">
+      <c r="Y48" s="104">
         <v>56</v>
       </c>
-      <c r="Z48" s="127">
+      <c r="Z48" s="104">
         <v>50</v>
       </c>
     </row>
@@ -7541,28 +7541,28 @@
       <c r="G49" s="46">
         <v>70</v>
       </c>
-      <c r="I49" s="113">
+      <c r="I49" s="90">
         <v>90</v>
       </c>
-      <c r="J49" s="113">
+      <c r="J49" s="90">
         <v>94</v>
       </c>
-      <c r="K49" s="113">
+      <c r="K49" s="90">
         <v>85</v>
       </c>
-      <c r="L49" s="113">
+      <c r="L49" s="90">
         <v>94</v>
       </c>
-      <c r="N49" s="113">
+      <c r="N49" s="90">
         <v>79</v>
       </c>
-      <c r="O49" s="113">
+      <c r="O49" s="90">
         <v>62</v>
       </c>
-      <c r="P49" s="113">
+      <c r="P49" s="90">
         <v>67</v>
       </c>
-      <c r="Q49" s="113">
+      <c r="Q49" s="90">
         <v>70</v>
       </c>
       <c r="T49" s="1" t="s">
@@ -7574,16 +7574,16 @@
       <c r="V49" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="W49" s="128">
+      <c r="W49" s="105">
         <v>90</v>
       </c>
-      <c r="X49" s="128">
+      <c r="X49" s="105">
         <v>94</v>
       </c>
-      <c r="Y49" s="128">
+      <c r="Y49" s="105">
         <v>85</v>
       </c>
-      <c r="Z49" s="128">
+      <c r="Z49" s="105">
         <v>94</v>
       </c>
     </row>
@@ -7642,16 +7642,16 @@
       <c r="V50" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="W50" s="129">
+      <c r="W50" s="106">
         <v>69</v>
       </c>
-      <c r="X50" s="129">
+      <c r="X50" s="106">
         <v>72</v>
       </c>
-      <c r="Y50" s="129">
+      <c r="Y50" s="106">
         <v>61</v>
       </c>
-      <c r="Z50" s="129">
+      <c r="Z50" s="106">
         <v>74</v>
       </c>
     </row>
@@ -7673,6 +7673,338 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEEE37E-912B-4737-A7D1-5910E79F6880}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
+    <col min="4" max="7" width="4" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
+    <col min="9" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="1.85546875" style="1" customWidth="1"/>
+    <col min="14" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="12.7109375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="71">
+        <v>1</v>
+      </c>
+      <c r="E2" s="71">
+        <v>2</v>
+      </c>
+      <c r="F2" s="71">
+        <v>3</v>
+      </c>
+      <c r="G2" s="71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="12">
+        <v>86</v>
+      </c>
+      <c r="E3" s="12">
+        <v>77</v>
+      </c>
+      <c r="F3" s="12">
+        <v>79</v>
+      </c>
+      <c r="G3" s="12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="12">
+        <v>57</v>
+      </c>
+      <c r="E4" s="12">
+        <v>67</v>
+      </c>
+      <c r="F4" s="12">
+        <v>53</v>
+      </c>
+      <c r="G4" s="12">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="12">
+        <v>79</v>
+      </c>
+      <c r="E5" s="12">
+        <v>62</v>
+      </c>
+      <c r="F5" s="12">
+        <v>67</v>
+      </c>
+      <c r="G5" s="12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="12">
+        <v>63</v>
+      </c>
+      <c r="E6" s="12">
+        <v>68</v>
+      </c>
+      <c r="F6" s="12">
+        <v>64</v>
+      </c>
+      <c r="G6" s="12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="12">
+        <v>68</v>
+      </c>
+      <c r="E7" s="12">
+        <v>75</v>
+      </c>
+      <c r="F7" s="12">
+        <v>58</v>
+      </c>
+      <c r="G7" s="12">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="12">
+        <v>73</v>
+      </c>
+      <c r="E8" s="12">
+        <v>70</v>
+      </c>
+      <c r="F8" s="12">
+        <v>67</v>
+      </c>
+      <c r="G8" s="12">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="12">
+        <v>76</v>
+      </c>
+      <c r="E9" s="12">
+        <v>90</v>
+      </c>
+      <c r="F9" s="12">
+        <v>89</v>
+      </c>
+      <c r="G9" s="12">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="12">
+        <v>46</v>
+      </c>
+      <c r="E10" s="12">
+        <v>52</v>
+      </c>
+      <c r="F10" s="12">
+        <v>58</v>
+      </c>
+      <c r="G10" s="12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="12">
+        <v>68</v>
+      </c>
+      <c r="E11" s="12">
+        <v>71</v>
+      </c>
+      <c r="F11" s="12">
+        <v>78</v>
+      </c>
+      <c r="G11" s="12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="12">
+        <v>47</v>
+      </c>
+      <c r="E12" s="12">
+        <v>49</v>
+      </c>
+      <c r="F12" s="12">
+        <v>56</v>
+      </c>
+      <c r="G12" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="12">
+        <v>90</v>
+      </c>
+      <c r="E13" s="12">
+        <v>94</v>
+      </c>
+      <c r="F13" s="12">
+        <v>85</v>
+      </c>
+      <c r="G13" s="12">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="12">
+        <v>69</v>
+      </c>
+      <c r="E14" s="12">
+        <v>72</v>
+      </c>
+      <c r="F14" s="12">
+        <v>61</v>
+      </c>
+      <c r="G14" s="12">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C5:AY51"/>
   <sheetViews>
@@ -7817,7 +8149,7 @@
       <c r="S7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="105" t="s">
+      <c r="U7" s="126" t="s">
         <v>37</v>
       </c>
       <c r="V7" s="8" t="s">
@@ -7829,7 +8161,7 @@
       <c r="X7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" s="105" t="s">
+      <c r="Z7" s="126" t="s">
         <v>37</v>
       </c>
       <c r="AA7" s="8" t="s">
@@ -7861,7 +8193,7 @@
       <c r="S8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="105"/>
+      <c r="U8" s="126"/>
       <c r="V8" s="14" t="s">
         <v>26</v>
       </c>
@@ -7871,7 +8203,7 @@
       <c r="X8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" s="105"/>
+      <c r="Z8" s="126"/>
       <c r="AA8" s="14" t="s">
         <v>26</v>
       </c>
@@ -7901,7 +8233,7 @@
       <c r="S9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="U9" s="106" t="s">
+      <c r="U9" s="127" t="s">
         <v>38</v>
       </c>
       <c r="V9" s="11" t="s">
@@ -7913,7 +8245,7 @@
       <c r="X9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Z9" s="106" t="s">
+      <c r="Z9" s="127" t="s">
         <v>38</v>
       </c>
       <c r="AA9" s="11" t="s">
@@ -7936,7 +8268,7 @@
       <c r="S10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="U10" s="106"/>
+      <c r="U10" s="127"/>
       <c r="V10" s="14" t="s">
         <v>28</v>
       </c>
@@ -7946,7 +8278,7 @@
       <c r="X10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Z10" s="106"/>
+      <c r="Z10" s="127"/>
       <c r="AA10" s="14" t="s">
         <v>28</v>
       </c>
@@ -8036,24 +8368,24 @@
       </c>
     </row>
     <row r="26" spans="7:43" x14ac:dyDescent="0.25">
-      <c r="AB26" s="107" t="s">
+      <c r="AB26" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="AC26" s="107"/>
-      <c r="AD26" s="107"/>
-      <c r="AE26" s="107"/>
-      <c r="AH26" s="107" t="s">
+      <c r="AC26" s="125"/>
+      <c r="AD26" s="125"/>
+      <c r="AE26" s="125"/>
+      <c r="AH26" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="AI26" s="107"/>
-      <c r="AJ26" s="107"/>
-      <c r="AK26" s="107"/>
-      <c r="AN26" s="107" t="s">
+      <c r="AI26" s="125"/>
+      <c r="AJ26" s="125"/>
+      <c r="AK26" s="125"/>
+      <c r="AN26" s="125" t="s">
         <v>119</v>
       </c>
-      <c r="AO26" s="107"/>
-      <c r="AP26" s="107"/>
-      <c r="AQ26" s="107"/>
+      <c r="AO26" s="125"/>
+      <c r="AP26" s="125"/>
+      <c r="AQ26" s="125"/>
     </row>
     <row r="27" spans="7:43" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
@@ -8182,7 +8514,7 @@
       <c r="AE28" s="10">
         <v>24.39</v>
       </c>
-      <c r="AG28" s="105" t="s">
+      <c r="AG28" s="126" t="s">
         <v>117</v>
       </c>
       <c r="AH28" s="8">
@@ -8197,7 +8529,7 @@
       <c r="AK28" s="10">
         <v>24.39</v>
       </c>
-      <c r="AM28" s="105" t="s">
+      <c r="AM28" s="126" t="s">
         <v>117</v>
       </c>
       <c r="AN28" s="8">
@@ -8268,7 +8600,7 @@
       <c r="AE29" s="13">
         <v>21.45</v>
       </c>
-      <c r="AG29" s="105"/>
+      <c r="AG29" s="126"/>
       <c r="AH29" s="11">
         <v>24.21</v>
       </c>
@@ -8281,7 +8613,7 @@
       <c r="AK29" s="13">
         <v>21.45</v>
       </c>
-      <c r="AM29" s="105"/>
+      <c r="AM29" s="126"/>
       <c r="AN29" s="11">
         <v>24.21</v>
       </c>
@@ -8350,7 +8682,7 @@
       <c r="AE30" s="13">
         <v>32.74</v>
       </c>
-      <c r="AG30" s="105"/>
+      <c r="AG30" s="126"/>
       <c r="AH30" s="11">
         <v>26.88</v>
       </c>
@@ -8363,7 +8695,7 @@
       <c r="AK30" s="13">
         <v>32.74</v>
       </c>
-      <c r="AM30" s="105"/>
+      <c r="AM30" s="126"/>
       <c r="AN30" s="14">
         <v>26.88</v>
       </c>
@@ -8411,7 +8743,7 @@
       <c r="AE31" s="13">
         <v>24.21</v>
       </c>
-      <c r="AG31" s="105" t="s">
+      <c r="AG31" s="126" t="s">
         <v>116</v>
       </c>
       <c r="AH31" s="8">
@@ -8426,7 +8758,7 @@
       <c r="AK31" s="10">
         <v>24.21</v>
       </c>
-      <c r="AM31" s="105" t="s">
+      <c r="AM31" s="126" t="s">
         <v>116</v>
       </c>
       <c r="AN31" s="11">
@@ -8476,7 +8808,7 @@
       <c r="AE32" s="13">
         <v>25.67</v>
       </c>
-      <c r="AG32" s="105"/>
+      <c r="AG32" s="126"/>
       <c r="AH32" s="11">
         <v>23.4</v>
       </c>
@@ -8489,7 +8821,7 @@
       <c r="AK32" s="13">
         <v>25.67</v>
       </c>
-      <c r="AM32" s="105"/>
+      <c r="AM32" s="126"/>
       <c r="AN32" s="11">
         <v>23.4</v>
       </c>
@@ -8537,7 +8869,7 @@
       <c r="AE33" s="16">
         <v>23.42</v>
       </c>
-      <c r="AG33" s="105"/>
+      <c r="AG33" s="126"/>
       <c r="AH33" s="14">
         <v>23.35</v>
       </c>
@@ -8550,7 +8882,7 @@
       <c r="AK33" s="16">
         <v>23.42</v>
       </c>
-      <c r="AM33" s="105"/>
+      <c r="AM33" s="126"/>
       <c r="AN33" s="14">
         <v>23.35</v>
       </c>
@@ -8671,7 +9003,7 @@
       <c r="AE37" s="10">
         <v>24.39</v>
       </c>
-      <c r="AG37" s="105" t="s">
+      <c r="AG37" s="126" t="s">
         <v>42</v>
       </c>
       <c r="AH37" s="8">
@@ -8686,7 +9018,7 @@
       <c r="AK37" s="10">
         <v>24.39</v>
       </c>
-      <c r="AM37" s="106" t="s">
+      <c r="AM37" s="127" t="s">
         <v>42</v>
       </c>
       <c r="AN37" s="8">
@@ -8724,7 +9056,7 @@
       <c r="AE38" s="13">
         <v>21.45</v>
       </c>
-      <c r="AG38" s="105"/>
+      <c r="AG38" s="126"/>
       <c r="AH38" s="11">
         <v>24.21</v>
       </c>
@@ -8737,7 +9069,7 @@
       <c r="AK38" s="13">
         <v>21.45</v>
       </c>
-      <c r="AM38" s="106"/>
+      <c r="AM38" s="127"/>
       <c r="AN38" s="11">
         <v>24.21</v>
       </c>
@@ -8773,7 +9105,7 @@
       <c r="AE39" s="13">
         <v>32.74</v>
       </c>
-      <c r="AG39" s="105"/>
+      <c r="AG39" s="126"/>
       <c r="AH39" s="11">
         <v>26.88</v>
       </c>
@@ -8786,7 +9118,7 @@
       <c r="AK39" s="13">
         <v>32.74</v>
       </c>
-      <c r="AM39" s="106"/>
+      <c r="AM39" s="127"/>
       <c r="AN39" s="14">
         <v>26.88</v>
       </c>
@@ -8822,7 +9154,7 @@
       <c r="AE40" s="13">
         <v>24.21</v>
       </c>
-      <c r="AG40" s="105" t="s">
+      <c r="AG40" s="126" t="s">
         <v>43</v>
       </c>
       <c r="AH40" s="8">
@@ -8837,7 +9169,7 @@
       <c r="AK40" s="10">
         <v>24.21</v>
       </c>
-      <c r="AM40" s="106" t="s">
+      <c r="AM40" s="127" t="s">
         <v>43</v>
       </c>
       <c r="AN40" s="11">
@@ -8875,7 +9207,7 @@
       <c r="AE41" s="13">
         <v>25.67</v>
       </c>
-      <c r="AG41" s="105"/>
+      <c r="AG41" s="126"/>
       <c r="AH41" s="11">
         <v>23.4</v>
       </c>
@@ -8888,7 +9220,7 @@
       <c r="AK41" s="13">
         <v>25.67</v>
       </c>
-      <c r="AM41" s="106"/>
+      <c r="AM41" s="127"/>
       <c r="AN41" s="11">
         <v>23.4</v>
       </c>
@@ -8924,7 +9256,7 @@
       <c r="AE42" s="16">
         <v>23.42</v>
       </c>
-      <c r="AG42" s="105"/>
+      <c r="AG42" s="126"/>
       <c r="AH42" s="14">
         <v>23.35</v>
       </c>
@@ -8937,7 +9269,7 @@
       <c r="AK42" s="16">
         <v>23.42</v>
       </c>
-      <c r="AM42" s="106"/>
+      <c r="AM42" s="127"/>
       <c r="AN42" s="14">
         <v>23.35</v>
       </c>
@@ -9439,11 +9771,6 @@
     <sortCondition ref="H27:H51"/>
   </sortState>
   <mergeCells count="15">
-    <mergeCell ref="AN26:AQ26"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="AG40:AG42"/>
     <mergeCell ref="AM40:AM42"/>
     <mergeCell ref="AG31:AG33"/>
@@ -9454,13 +9781,18 @@
     <mergeCell ref="AG37:AG39"/>
     <mergeCell ref="AM37:AM39"/>
     <mergeCell ref="AH26:AK26"/>
+    <mergeCell ref="AN26:AQ26"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="Z9:Z10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:Y8"/>
   <sheetViews>
@@ -9477,36 +9809,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="G2" s="108" t="s">
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="G2" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="L2" s="108" t="s">
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="L2" s="128" t="s">
         <v>120</v>
       </c>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="Q2" s="109" t="s">
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
+      <c r="Q2" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="V2" s="89" t="s">
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="V2" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="109"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
@@ -9677,7 +10009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B883F1-1F0C-4524-B73F-E7D1A0CFC916}">
   <dimension ref="B2:X6"/>
   <sheetViews>
@@ -9777,7 +10109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F787B73C-D5B7-4C11-BF48-18C26E72EF85}">
   <dimension ref="A2:T29"/>
   <sheetViews>
@@ -9798,18 +10130,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="L2" s="89" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="L2" s="109" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
     </row>
     <row r="3" spans="1:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="82" t="s">
@@ -9825,12 +10157,12 @@
         <v>148</v>
       </c>
       <c r="F3" s="79"/>
-      <c r="G3" s="108" t="s">
+      <c r="G3" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
       <c r="K3" s="79"/>
       <c r="L3" s="82" t="s">
         <v>145</v>
@@ -10084,18 +10416,18 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="L12" s="89" t="s">
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="L12" s="109" t="s">
         <v>150</v>
       </c>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
     </row>
     <row r="13" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="82" t="s">
@@ -10111,12 +10443,12 @@
         <v>148</v>
       </c>
       <c r="F13" s="79"/>
-      <c r="G13" s="108" t="s">
+      <c r="G13" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="H13" s="108"/>
-      <c r="I13" s="108"/>
-      <c r="J13" s="108"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
       <c r="K13" s="79"/>
       <c r="L13" s="82" t="s">
         <v>145</v>
@@ -10131,12 +10463,12 @@
         <v>148</v>
       </c>
       <c r="P13" s="79"/>
-      <c r="Q13" s="108" t="s">
+      <c r="Q13" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="R13" s="108"/>
-      <c r="S13" s="108"/>
-      <c r="T13" s="108"/>
+      <c r="R13" s="128"/>
+      <c r="S13" s="128"/>
+      <c r="T13" s="128"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="46">
@@ -10424,18 +10756,18 @@
       <c r="T19" s="81"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89"/>
-      <c r="L22" s="89" t="s">
+      <c r="C22" s="109"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
+      <c r="L22" s="109" t="s">
         <v>150</v>
       </c>
-      <c r="M22" s="89"/>
-      <c r="N22" s="89"/>
-      <c r="O22" s="89"/>
+      <c r="M22" s="109"/>
+      <c r="N22" s="109"/>
+      <c r="O22" s="109"/>
     </row>
     <row r="23" spans="2:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="82" t="s">
@@ -10451,12 +10783,12 @@
         <v>148</v>
       </c>
       <c r="F23" s="79"/>
-      <c r="G23" s="108" t="s">
+      <c r="G23" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="H23" s="108"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="108"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="128"/>
+      <c r="J23" s="128"/>
       <c r="K23" s="79"/>
       <c r="L23" s="82" t="s">
         <v>145</v>
@@ -10471,12 +10803,12 @@
         <v>148</v>
       </c>
       <c r="P23" s="79"/>
-      <c r="Q23" s="108" t="s">
+      <c r="Q23" s="128" t="s">
         <v>151</v>
       </c>
-      <c r="R23" s="108"/>
-      <c r="S23" s="108"/>
-      <c r="T23" s="108"/>
+      <c r="R23" s="128"/>
+      <c r="S23" s="128"/>
+      <c r="T23" s="128"/>
     </row>
     <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="46">
@@ -10837,17 +11169,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="L12:O12"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="Q13:T13"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="L22:O22"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="L12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>